<commit_message>
Coverage Drive Verification 1: <Coverage:73.60%>, <Goal of testplan:5…
</commit_message>
<xml_diff>
--- a/rkv_i2c_tb/doc/questa_vplan.xlsx
+++ b/rkv_i2c_tb/doc/questa_vplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DVT_Code\MyIIC\rkv_v2pro_i2c-RKV_I2C_TB_05\rkv_i2c_tb05\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE61DDAB-FE68-4F4A-85C9-F105E7C86AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824FCCB8-DCA1-4D6E-B723-FA52BC6C73A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
 rkv_i2c_master_start_byte_test_*
 i2c_master_tx_empty_intr_test_*
 i2c_master_sda_control_cg_test_*
-rkv_i2c_master_timeout_cg_test_*
+i2c_master_timeout_cg_test_*
 i2c_master_abrt_10b_rd_norstrt_test_*
 i2c_master_ss_cnt_test_*
 i2c_master_fs_cnt_test_*

</xml_diff>

<commit_message>
CDV 4: <Goal of testplan:%81.16>, <Coverage:%81.27>
</commit_message>
<xml_diff>
--- a/rkv_i2c_tb/doc/questa_vplan.xlsx
+++ b/rkv_i2c_tb/doc/questa_vplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DVT_Code\MyIIC\rkv_v2pro_i2c-RKV_I2C_TB_05\rkv_i2c_tb05\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824FCCB8-DCA1-4D6E-B723-FA52BC6C73A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D58657A-F826-4FC8-83D5-CBAE34BB24BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,7 +329,7 @@
 rkv_i2c_reg_hw_reset_test_*
 i2c_master_abrt_7b_addr_noack_test_*
 i2c_master_abrt_sbyte_norstrt_test_*
-rkv_i2c_master_start_byte_test_*
+i2c_master_start_byte_test_*
 i2c_master_tx_empty_intr_test_*
 i2c_master_sda_control_cg_test_*
 i2c_master_timeout_cg_test_*
@@ -337,7 +337,7 @@
 i2c_master_ss_cnt_test_*
 i2c_master_fs_cnt_test_*
 i2c_master_hs_cnt_test_*
-rkv_i2c_master_hs_master_code_test_*</t>
+i2c_master_hs_master_code_test_*</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>

</xml_diff>